<commit_message>
Update Urenverantwoording and put together STDs
</commit_message>
<xml_diff>
--- a/Administratie/Planning/Uren verantwoording.xlsx
+++ b/Administratie/Planning/Uren verantwoording.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17520"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hogeschoolutrecht.sharepoint.com/sites/tekteamone/Gedeelde  documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arco/Documents/TekTeamOne/Administratie/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="7_{8F492140-3DC6-421A-86DF-53F185B28202}" xr6:coauthVersionLast="10" xr6:coauthVersionMax="10" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="435" windowWidth="33600" windowHeight="19785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19740"/>
   </bookViews>
   <sheets>
     <sheet name="Urenverantwoording" sheetId="1" r:id="rId1"/>
@@ -19,17 +18,20 @@
     <sheet name="Dagindeling" sheetId="5" r:id="rId4"/>
     <sheet name="Opties" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="79">
   <si>
     <t>Taak</t>
   </si>
@@ -154,6 +156,18 @@
     <t>Bestuderen software architecture en opzet eigen software architecture</t>
   </si>
   <si>
+    <t>STD's maken</t>
+  </si>
+  <si>
+    <t>Objectlijst maken</t>
+  </si>
+  <si>
+    <t>Opmaak &amp; Indeling</t>
+  </si>
+  <si>
+    <t>Opzet onderzoek</t>
+  </si>
+  <si>
     <t>Gepland</t>
   </si>
   <si>
@@ -179,9 +193,6 @@
   </si>
   <si>
     <t>Presentatie</t>
-  </si>
-  <si>
-    <t>Opmaak &amp; Indeling</t>
   </si>
   <si>
     <t>Bronvermelding</t>
@@ -246,17 +257,29 @@
   </si>
   <si>
     <t>Onderdeel</t>
+  </si>
+  <si>
+    <t>STD's afmaken</t>
+  </si>
+  <si>
+    <t>Bedenken welke RTOS'en er gebruikt gaan worden</t>
+  </si>
+  <si>
+    <t>Administratie van de afgelopen tijd samengevoegd tot totale tijd</t>
+  </si>
+  <si>
+    <t>STD's samenvoegen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,28 +393,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -406,7 +429,7 @@
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -418,10 +441,10 @@
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -430,7 +453,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -448,7 +471,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -460,7 +483,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -469,7 +492,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -484,7 +507,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,13 +516,13 @@
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,121 +530,121 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -714,10 +737,10 @@
     <xf numFmtId="16" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -743,8 +766,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="62">
     <dxf>
@@ -1642,24 +1665,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1710,7 +1733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1727,7 +1750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1744,7 +1767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1761,7 +1784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1778,7 +1801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1795,7 +1818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1812,7 +1835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1846,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1863,7 +1886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1897,7 +1920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1914,7 +1937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1931,7 +1954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1948,7 +1971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +1988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1982,7 +2005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1999,7 +2022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2016,7 +2039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2033,7 +2056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2050,7 +2073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -2067,7 +2090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2084,7 +2107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2101,7 +2124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2118,7 +2141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2135,7 +2158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2152,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2169,7 +2192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2186,7 +2209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2203,7 +2226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2220,7 +2243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2237,7 +2260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2254,7 +2277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2271,7 +2294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2288,7 +2311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2322,7 +2345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2339,7 +2362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2356,7 +2379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2373,7 +2396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2407,7 +2430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2441,7 +2464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2458,7 +2481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2475,7 +2498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2492,7 +2515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2509,7 +2532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2526,7 +2549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2543,7 +2566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2560,7 +2583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2577,7 +2600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2594,7 +2617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -2611,7 +2634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -2628,7 +2651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2662,7 +2685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -2679,7 +2702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -2696,7 +2719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -2713,7 +2736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -2747,7 +2770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -2764,7 +2787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -2781,7 +2804,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -2798,7 +2821,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -2815,7 +2838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -2832,7 +2855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -2849,7 +2872,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2866,7 +2889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2883,7 +2906,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -2900,7 +2923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -2917,7 +2940,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -2934,7 +2957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -2951,7 +2974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -2968,7 +2991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -2983,6 +3006,278 @@
       </c>
       <c r="E78" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>39</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81">
+        <v>6</v>
+      </c>
+      <c r="D81" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E83" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>43</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3">
+        <v>42668</v>
+      </c>
+      <c r="E86" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87">
+        <v>4.5</v>
+      </c>
+      <c r="D87" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88">
+        <v>2.5</v>
+      </c>
+      <c r="D88" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89">
+        <v>4.5</v>
+      </c>
+      <c r="D89" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E89" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90">
+        <v>4.5</v>
+      </c>
+      <c r="D90" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E90" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>55</v>
+      </c>
+      <c r="B91" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <v>42669</v>
+      </c>
+      <c r="E92" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" s="3">
+        <v>42670</v>
+      </c>
+      <c r="E93" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>39</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>0.5</v>
+      </c>
+      <c r="D94" s="3">
+        <v>42670</v>
+      </c>
+      <c r="E94" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2990,7 +3285,7 @@
     <sortCondition ref="B2:B55"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>42614</formula1>
       <formula2>42923</formula2>
     </dataValidation>
@@ -3000,25 +3295,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Taken!$D$3:$D$7</xm:f>
           </x14:formula1>
           <xm:sqref>B4916:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Taken!$A$3:$A$44</xm:f>
           </x14:formula1>
           <xm:sqref>A4684:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Opties!$B$1:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B4915</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Opties!$A$1:$A$17</xm:f>
           </x14:formula1>
@@ -3031,51 +3326,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
         <f>SUMIF(Urenverantwoording!A2:A1048576,Taken!A3,Urenverantwoording!C2:C1048576)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3084,7 +3379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3093,7 +3388,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1">
+    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -3102,7 +3397,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="5" customFormat="1">
+    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -3111,7 +3406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="5" customFormat="1">
+    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -3120,23 +3415,23 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="5" customFormat="1">
+    <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5">
         <f>SUM(C3:C8)</f>
-        <v>152.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="5" customFormat="1">
+        <v>153.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
@@ -3145,10 +3440,10 @@
       </c>
       <c r="C11" s="5">
         <f>SUMIF(Urenverantwoording!A2:A1048576,Taken!A11,Urenverantwoording!C2:C1048576)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -3160,7 +3455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -3172,9 +3467,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -3184,9 +3479,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -3196,9 +3491,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>17</v>
@@ -3208,9 +3503,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>14</v>
@@ -3220,21 +3515,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" s="5">
         <f>SUMIF(Urenverantwoording!$A$2:$A$1048576,Taken!A18,Urenverantwoording!$C$2:$C$1048576)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -3244,21 +3539,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>16</v>
       </c>
       <c r="C20" s="5">
         <f>SUMIF(Urenverantwoording!$A$2:$A$1048576,Taken!A20,Urenverantwoording!$C$2:$C$1048576)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -3268,18 +3563,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.5" customHeight="1">
+    <row r="22" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <f>SUM(B11:B22)</f>
@@ -3287,7 +3582,7 @@
       </c>
       <c r="C23">
         <f>SUM(C11:C21)</f>
-        <v>28.5</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3300,24 +3595,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="29" customFormat="1" ht="28.5">
+    <row r="1" spans="1:11" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="30"/>
       <c r="B1" s="38" t="s">
         <v>19</v>
@@ -3336,15 +3631,15 @@
       </c>
       <c r="I1" s="39"/>
       <c r="J1" s="29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -3355,36 +3650,36 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:11" ht="26.25">
+    <row r="3" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>16</v>
       </c>
@@ -3417,7 +3712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
@@ -3450,7 +3745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
@@ -3483,7 +3778,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
@@ -3516,7 +3811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>10</v>
       </c>
@@ -3549,7 +3844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
@@ -3582,9 +3877,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B10" s="17">
         <f>SUM(B4:B9)</f>
@@ -3619,9 +3914,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="27" thickBot="1">
+    <row r="11" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
@@ -3632,37 +3927,37 @@
       <c r="H11" s="36"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:11" ht="26.25">
+    <row r="12" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="9">
@@ -3694,7 +3989,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
@@ -3727,7 +4022,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>8</v>
       </c>
@@ -3743,7 +4038,7 @@
       </c>
       <c r="E15" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A15,Urenverantwoording!$B$2:$B$1048576,$D$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="9">
         <v>0</v>
@@ -3760,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -3801,7 +4096,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -3842,16 +4137,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
       </c>
       <c r="C18" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A18,Urenverantwoording!$B$2:$B$1048576,$B$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="9">
         <v>8</v>
@@ -3865,7 +4160,7 @@
       </c>
       <c r="G18" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A18,Urenverantwoording!$B$2:$B$1048576,$F$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="9">
         <v>8</v>
@@ -3883,9 +4178,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -3924,9 +4219,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B20" s="9">
         <v>0.5</v>
@@ -3965,37 +4260,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
       </c>
       <c r="C21" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A21,Urenverantwoording!$B$2:$B$1048576,$B$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="9">
         <v>3</v>
       </c>
       <c r="E21" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A21,Urenverantwoording!$B$2:$B$1048576,$D$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="9">
         <v>1</v>
       </c>
       <c r="G21" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A21,Urenverantwoording!$B$2:$B$1048576,$F$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="9">
         <v>3</v>
       </c>
       <c r="I21" s="15">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A21,Urenverantwoording!$B$2:$B$1048576,$H$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="8">
         <f>SUM(Dagindeling!C9,Dagindeling!E9,Dagindeling!G9,Dagindeling!I9,Dagindeling!K9)</f>
@@ -4006,9 +4301,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -4047,9 +4342,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B23" s="9">
         <v>1.5</v>
@@ -4088,7 +4383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -4097,28 +4392,28 @@
       </c>
       <c r="C24" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A24,Urenverantwoording!$B$2:$B$1048576,$B$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>1</v>
+        <v>11.5</v>
       </c>
       <c r="D24" s="9">
         <v>11</v>
       </c>
       <c r="E24" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A24,Urenverantwoording!$B$2:$B$1048576,$D$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F24" s="9">
         <v>8</v>
       </c>
       <c r="G24" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A24,Urenverantwoording!$B$2:$B$1048576,$F$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="H24" s="9">
         <v>11</v>
       </c>
       <c r="I24" s="15">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A24,Urenverantwoording!$B$2:$B$1048576,$H$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="J24" s="8">
         <f>SUM(Dagindeling!C2,Dagindeling!E2,Dagindeling!G2,Dagindeling!I2,Dagindeling!K2)</f>
@@ -4129,41 +4424,41 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B25" s="17">
-        <f>SUM(B13:B24)</f>
+        <f t="shared" ref="B25:I25" si="2">SUM(B13:B24)</f>
         <v>40</v>
       </c>
       <c r="C25" s="9">
-        <f>SUM(C13:C24)</f>
-        <v>12.5</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="D25" s="17">
-        <f>SUM(D13:D24)</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="E25" s="9">
-        <f>SUM(E13:E24)</f>
-        <v>3.5</v>
+        <f t="shared" si="2"/>
+        <v>16.5</v>
       </c>
       <c r="F25" s="17">
-        <f>SUM(F13:F24)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="G25" s="9">
-        <f>SUM(G13:G24)</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>22.5</v>
       </c>
       <c r="H25" s="17">
-        <f>SUM(H13:H24)</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="I25" s="9">
-        <f>SUM(I13:I24)</f>
-        <v>8.5</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="J25" s="8">
         <f>SUM(J16:J24)</f>
@@ -4174,9 +4469,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="27" thickBot="1">
+    <row r="26" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -4188,39 +4483,39 @@
       <c r="I26" s="36"/>
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:11" ht="26.25">
+    <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B28" s="9">
         <v>0</v>
@@ -4259,9 +4554,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
@@ -4300,7 +4595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -4341,7 +4636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
@@ -4382,9 +4677,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B32" s="9">
         <v>1.5</v>
@@ -4423,9 +4718,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -4464,7 +4759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>8</v>
       </c>
@@ -4504,40 +4799,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1">
+    <row r="35" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B35" s="17">
-        <f t="shared" ref="B35:I35" si="2">SUM(B27:B34)</f>
+        <f t="shared" ref="B35:I35" si="3">SUM(B27:B34)</f>
         <v>14.5</v>
       </c>
       <c r="C35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D35" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="E35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F35" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.5</v>
       </c>
       <c r="G35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H35" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J35" s="8">
@@ -4549,9 +4844,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="27" thickBot="1">
+    <row r="36" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B36" s="37"/>
       <c r="C36" s="37"/>
@@ -4563,39 +4858,39 @@
       <c r="I36" s="37"/>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:11" ht="26.25">
+    <row r="37" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B38" s="9">
         <v>2</v>
@@ -4634,9 +4929,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B39" s="9">
         <v>3</v>
@@ -4675,7 +4970,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
@@ -4716,7 +5011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>29</v>
       </c>
@@ -4757,9 +5052,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
@@ -4798,9 +5093,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B43" s="9">
         <v>3</v>
@@ -4839,36 +5134,36 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1">
+    <row r="44" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B44" s="17">
-        <f t="shared" ref="B44:H44" si="3">SUM(B37:B43)</f>
+        <f t="shared" ref="B44:H44" si="4">SUM(B37:B43)</f>
         <v>21</v>
       </c>
       <c r="C44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21.5</v>
       </c>
       <c r="E44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="G44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21.5</v>
       </c>
       <c r="I44" s="18">
@@ -4883,9 +5178,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="27" thickBot="1">
+    <row r="45" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B45" s="37"/>
       <c r="C45" s="37"/>
@@ -4896,112 +5191,112 @@
       <c r="H45" s="37"/>
       <c r="I45" s="37"/>
     </row>
-    <row r="46" spans="1:11" ht="26.25">
+    <row r="46" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="25" customFormat="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B47" s="24">
-        <f t="shared" ref="B47:I47" si="4">SUM(B25,B35,B44)</f>
+        <f t="shared" ref="B47:I47" si="5">SUM(B25,B35,B44)</f>
         <v>75.5</v>
       </c>
       <c r="C47" s="10">
-        <f t="shared" si="4"/>
-        <v>12.5</v>
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="D47" s="24">
-        <f t="shared" si="4"/>
-        <v>74.5</v>
-      </c>
-      <c r="E47" s="10">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
-      </c>
-      <c r="F47" s="24">
-        <f t="shared" si="4"/>
-        <v>75.5</v>
-      </c>
-      <c r="G47" s="10">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="H47" s="24">
-        <f t="shared" si="4"/>
-        <v>74.5</v>
-      </c>
-      <c r="I47" s="10">
-        <f t="shared" si="4"/>
-        <v>8.5</v>
-      </c>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-    </row>
-    <row r="48" spans="1:11" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A48" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="27">
-        <f t="shared" ref="B48:I48" si="5">SUM(B47,B10)</f>
-        <v>75.5</v>
-      </c>
-      <c r="C48" s="27">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-      <c r="D48" s="27">
         <f t="shared" si="5"/>
         <v>74.5</v>
       </c>
-      <c r="E48" s="27">
+      <c r="E47" s="10">
         <f t="shared" si="5"/>
-        <v>39.5</v>
-      </c>
-      <c r="F48" s="27">
+        <v>16.5</v>
+      </c>
+      <c r="F47" s="24">
         <f t="shared" si="5"/>
         <v>75.5</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G47" s="10">
         <f t="shared" si="5"/>
-        <v>54</v>
-      </c>
-      <c r="H48" s="27">
+        <v>22.5</v>
+      </c>
+      <c r="H47" s="24">
         <f t="shared" si="5"/>
         <v>74.5</v>
       </c>
+      <c r="I47" s="10">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+    </row>
+    <row r="48" spans="1:11" s="25" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="27">
+        <f t="shared" ref="B48:I48" si="6">SUM(B47,B10)</f>
+        <v>75.5</v>
+      </c>
+      <c r="C48" s="27">
+        <f t="shared" si="6"/>
+        <v>60.5</v>
+      </c>
+      <c r="D48" s="27">
+        <f t="shared" si="6"/>
+        <v>74.5</v>
+      </c>
+      <c r="E48" s="27">
+        <f t="shared" si="6"/>
+        <v>52.5</v>
+      </c>
+      <c r="F48" s="27">
+        <f t="shared" si="6"/>
+        <v>75.5</v>
+      </c>
+      <c r="G48" s="27">
+        <f t="shared" si="6"/>
+        <v>67.5</v>
+      </c>
+      <c r="H48" s="27">
+        <f t="shared" si="6"/>
+        <v>74.5</v>
+      </c>
       <c r="I48" s="28">
-        <f t="shared" si="5"/>
-        <v>40.5</v>
-      </c>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5200,7 +5495,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Opties!$A$1:$A$17</xm:f>
           </x14:formula1>
@@ -5213,47 +5508,47 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE4" sqref="AE4"/>
+      <selection pane="topRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="4.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="30" width="4.42578125" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="4.5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="30" width="4.5" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="40">
         <f>DATE(2016,10,24)</f>
@@ -5333,7 +5628,7 @@
       </c>
       <c r="AN1" s="40"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -5422,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -5517,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5616,9 +5911,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B5" s="8">
         <f t="shared" si="0"/>
@@ -5711,9 +6006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B6" s="8">
         <f t="shared" si="0"/>
@@ -5796,9 +6091,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" s="8">
         <f t="shared" si="0"/>
@@ -5887,9 +6182,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8">
         <f t="shared" si="0"/>
@@ -5972,9 +6267,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8">
         <f t="shared" si="0"/>
@@ -6059,9 +6354,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B10" s="8">
         <f t="shared" si="0"/>
@@ -6148,9 +6443,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B11" s="8">
         <f t="shared" si="0"/>
@@ -6237,9 +6532,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B12" s="8">
         <f t="shared" si="0"/>
@@ -6326,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C13" s="8">
         <f>SUM(C2:C12)</f>
         <v>32</v>
@@ -6480,7 +6775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -6520,7 +6815,7 @@
       <c r="AM14" s="8"/>
       <c r="AN14" s="8"/>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -6560,7 +6855,7 @@
       <c r="AM15" s="8"/>
       <c r="AN15" s="8"/>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -6600,7 +6895,7 @@
       <c r="AM16" s="8"/>
       <c r="AN16" s="8"/>
     </row>
-    <row r="17" spans="3:40">
+    <row r="17" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -6640,7 +6935,7 @@
       <c r="AM17" s="8"/>
       <c r="AN17" s="8"/>
     </row>
-    <row r="18" spans="3:40">
+    <row r="18" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -6682,6 +6977,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -6694,13 +6996,6 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
@@ -6828,19 +7123,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -6848,7 +7143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6856,7 +7151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6864,7 +7159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -6872,69 +7167,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Onderzoeksverslag and update Urenverantwoording
</commit_message>
<xml_diff>
--- a/Administratie/Planning/Uren verantwoording.xlsx
+++ b/Administratie/Planning/Uren verantwoording.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19740"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Urenverantwoording" sheetId="1" r:id="rId1"/>
@@ -1674,9 +1674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2920,7 +2920,7 @@
         <v>6</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D73" s="3">
         <v>42667</v>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="C7" s="5">
         <f>SUMIF(Urenverantwoording!A2:A1048576,Taken!A7,Urenverantwoording!C2:C1048576)</f>
-        <v>22</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="C9" s="5">
         <f>SUM(C3:C8)</f>
-        <v>153.5</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -3638,9 +3638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="E13" s="9">
         <f>SUMIFS(Urenverantwoording!$C$2:$C$1048576,Urenverantwoording!$A$2:$A$1048576,A13,Urenverantwoording!$B$2:$B$1048576,$D$1,Urenverantwoording!$D$2:$D$1048576,"&gt;=" &amp; DATE(2016,10,24),Urenverantwoording!$D$2:$D$1048576,"&lt;" &amp; DATE(2016,10,31))</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F13" s="9">
         <v>0</v>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>23.5</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" si="2"/>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="E47" s="10">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>23.5</v>
       </c>
       <c r="F47" s="24">
         <f t="shared" si="5"/>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="E48" s="27">
         <f t="shared" si="6"/>
-        <v>59</v>
+        <v>59.5</v>
       </c>
       <c r="F48" s="27">
         <f t="shared" si="6"/>

</xml_diff>